<commit_message>
add excelutil and properties util
</commit_message>
<xml_diff>
--- a/src/test/resources/config.xlsx
+++ b/src/test/resources/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Calc-engine-dataTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020C7786-6A08-492F-BF12-0AFA80BC0C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403A563E-1A4E-4630-9667-2945B5AED9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51034034-E55F-4D7C-B166-9B0BA830FBBD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>UAT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,30 @@
   </si>
   <si>
     <t>dbInstance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -446,7 +470,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -473,6 +497,9 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -481,6 +508,9 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -489,6 +519,9 @@
       <c r="B4" s="1">
         <v>62658</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -497,6 +530,9 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -505,6 +541,9 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -512,6 +551,9 @@
       </c>
       <c r="B7" t="s">
         <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all config related read
</commit_message>
<xml_diff>
--- a/src/test/resources/config.xlsx
+++ b/src/test/resources/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Calc-engine-dataTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403A563E-1A4E-4630-9667-2945B5AED9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA9F12F-676E-41EE-BD36-0CCEAEE180E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51034034-E55F-4D7C-B166-9B0BA830FBBD}"/>
+    <workbookView xWindow="6255" yWindow="705" windowWidth="18885" windowHeight="14220" xr2:uid="{51034034-E55F-4D7C-B166-9B0BA830FBBD}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>UAT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +101,13 @@
   <si>
     <t>fff</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbdriver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.microsoft.sqlserver.jdbc.SQLServerDriver</t>
   </si>
 </sst>
 </file>
@@ -467,16 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5633D7A0-07D6-48CF-9E67-4C834FBD48A7}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="4" width="33.75" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="4" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -554,6 +562,14 @@
       </c>
       <c r="C7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>